<commit_message>
Update to include data of 2021-02-23.
</commit_message>
<xml_diff>
--- a/ars_data_raw.xlsx
+++ b/ars_data_raw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="22">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">From here from 2021-02-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: 2021-02-23</t>
   </si>
   <si>
     <t xml:space="preserve">Länge für Einheit (cm)</t>
@@ -272,15 +275,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J168"/>
+  <dimension ref="A1:J180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E80" activeCellId="0" sqref="E80"/>
+      <selection pane="bottomLeft" activeCell="E176" activeCellId="0" sqref="E176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.77"/>
@@ -3241,13 +3244,6 @@
       <c r="G149" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I149" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J149" s="0" t="n">
-        <f aca="false">26-8.9</f>
-        <v>17.1</v>
-      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
@@ -3271,12 +3267,6 @@
       <c r="G150" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="I150" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J150" s="0" t="n">
-        <v>150</v>
-      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
@@ -3300,13 +3290,6 @@
       <c r="G151" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="I151" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J151" s="0" t="n">
-        <f aca="false">J150 / J149</f>
-        <v>8.7719298245614</v>
-      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
@@ -3330,12 +3313,6 @@
       <c r="G152" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="I152" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J152" s="0" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
@@ -3359,12 +3336,6 @@
       <c r="G153" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="I153" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J153" s="0" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
@@ -3388,21 +3359,6 @@
       <c r="G154" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="I154" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J154" s="3" t="n">
-        <v>18.1</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J155" s="1" t="n">
-        <f aca="false">(J154-J152)*J151+J153</f>
-        <v>130.701754385965</v>
-      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
@@ -3472,10 +3428,6 @@
       <c r="G158" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="I158" s="0" t="n">
-        <f aca="false">50000/55</f>
-        <v>909.090909090909</v>
-      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
@@ -3499,10 +3451,6 @@
       <c r="G159" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="I159" s="0" t="n">
-        <f aca="false">50000 + 909 * 9</f>
-        <v>58181</v>
-      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
@@ -3526,10 +3474,6 @@
       <c r="G160" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="I160" s="0" t="n">
-        <f aca="false">909*8</f>
-        <v>7272</v>
-      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
@@ -3690,6 +3634,176 @@
       </c>
       <c r="G168" s="0" t="n">
         <v>130</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I169" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J169" s="0" t="n">
+        <f aca="false">26.4-6</f>
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>7819</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="I170" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J170" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>10664</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="I171" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J171" s="0" t="n">
+        <f aca="false">J170 / J169</f>
+        <v>0.490196078431373</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>95972</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="I172" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J172" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>153555</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="I173" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J173" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>86730</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J174" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>53318</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J175" s="1" t="n">
+        <f aca="false">(J174-J172)*J171+J173</f>
+        <v>6.47058823529412</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I178" s="0" t="n">
+        <f aca="false">50000/55</f>
+        <v>909.090909090909</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I179" s="0" t="n">
+        <f aca="false">50000 + 909 * 9</f>
+        <v>58181</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I180" s="0" t="n">
+        <f aca="false">909*8</f>
+        <v>7272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>